<commit_message>
Add Hasil Ujian relationship to UserModel and update UI components Hasil Ujian Peserta
</commit_message>
<xml_diff>
--- a/PBLSEM4/public/template_user.xlsx
+++ b/PBLSEM4/public/template_user.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\SIPINTA\PBLSEM4\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Polinema\STUDI KAMPUS\SEMESTER 4\WEB\PBLSEM4\PBLSEM4\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547736F0-0E3F-4F6C-B12D-BEE11FA52D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD9E0CD-D736-4EB0-BD99-477159A5C697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="12090" xr2:uid="{CF1C9569-87DC-4D3D-8CB6-AB1D3718DEE1}"/>
+    <workbookView minimized="1" xWindow="4046" yWindow="4046" windowWidth="18514" windowHeight="11280" xr2:uid="{CF1C9569-87DC-4D3D-8CB6-AB1D3718DEE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,16 +433,16 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="2" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.69140625" customWidth="1"/>
+    <col min="2" max="2" width="22.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -493,5 +493,6 @@
     <hyperlink ref="A2" r:id="rId1" xr:uid="{7A878FD0-F587-4F8F-9010-1A82B3D8A56A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>